<commit_message>
Updated tables to reflect new info
</commit_message>
<xml_diff>
--- a/VectorDataInExcel-2NF.xlsx
+++ b/VectorDataInExcel-2NF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Database\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{BD6218DC-6011-4F10-BEE8-85B92B991643}"/>
+  <xr:revisionPtr revIDLastSave="349" documentId="8_{9B9F850F-ADFF-4EEF-A28E-9D797F0D7DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{CC9D0C90-725D-4071-9364-688155112A55}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7DCE2BE0-953A-4365-ADEC-B2ECAC53B523}"/>
   </bookViews>
@@ -514,15 +514,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1175162</xdr:colOff>
+      <xdr:colOff>1175161</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>61851</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1373084</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>111331</xdr:rowOff>
+      <xdr:colOff>1385454</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>148441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -537,8 +537,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1175162" y="9896104"/>
-          <a:ext cx="197922" cy="2461656"/>
+          <a:off x="1175161" y="9896104"/>
+          <a:ext cx="210293" cy="1199902"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst/>
@@ -922,13 +922,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1063832</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>123701</xdr:rowOff>
+      <xdr:rowOff>123702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1138052</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>6185</xdr:rowOff>
+      <xdr:colOff>1150422</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -943,8 +943,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1063832" y="494805"/>
-          <a:ext cx="74220" cy="10644497"/>
+          <a:off x="1063832" y="494806"/>
+          <a:ext cx="86590" cy="11702142"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1191,6 +1191,64 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1191490</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>3958</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1401783</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>90548</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Left Brace 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43079B38-90E0-4668-A2A0-9DF08E07A85B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1191490" y="11322627"/>
+          <a:ext cx="210293" cy="1199902"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-NZ" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1496,10 +1554,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E72"/>
+  <dimension ref="B2:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,114 +1966,114 @@
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>55</v>
+      <c r="B59" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="11">
+        <v>152.75243237628899</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>5</v>
+      <c r="B60" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="10">
+        <v>-27.6047716895375</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C61" s="11">
-        <v>152.75243237628899</v>
+        <v>58</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C62" s="10">
-        <v>-27.6047716895375</v>
+        <v>60</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>59</v>
+      <c r="B63" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="7" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C65" s="11">
-        <v>8.9314404000248103E+19</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="10">
-        <v>8.9610180002248999E+19</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>51</v>
+      <c r="B67" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>66</v>
+      <c r="B68" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="C69" s="11">
+        <v>8.9314404000248103E+19</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+      <c r="C70" s="10">
+        <v>8.9610180002248999E+19</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C71" s="11">
-        <v>3.92</v>
+        <v>64</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C73" s="7" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>